<commit_message>
Changed Analysis and Statistics
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C221A950-6A03-4034-9416-2F0200C95837}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE045AE4-5FAF-4045-B90C-E95D1E1DD477}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,6 @@
     <sheet name="FinalDec" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="40">
   <si>
     <t>RMSE</t>
   </si>
@@ -328,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -356,7 +355,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,8 +396,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,30 +698,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1906,22 +1904,22 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="31" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -2870,22 +2868,22 @@
       <c r="S43" s="4"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="32" t="s">
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -3708,22 +3706,22 @@
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="28" t="s">
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="30"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="30"/>
+      <c r="L67" s="30"/>
+      <c r="M67" s="31"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -4586,30 +4584,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -5792,22 +5790,22 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="31" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -6756,22 +6754,22 @@
       <c r="S43" s="4"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="32" t="s">
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -7594,22 +7592,22 @@
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="28" t="s">
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="30"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="30"/>
+      <c r="L67" s="30"/>
+      <c r="M67" s="31"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -8472,30 +8470,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9678,22 +9676,22 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="31" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -10642,22 +10640,22 @@
       <c r="S43" s="4"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="32" t="s">
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -11480,22 +11478,22 @@
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="28" t="s">
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="30"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="30"/>
+      <c r="L67" s="30"/>
+      <c r="M67" s="31"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -12023,7 +12021,7 @@
       <c r="K80" s="19">
         <v>1.8111999999999999</v>
       </c>
-      <c r="L80" s="42">
+      <c r="L80" s="28">
         <v>5300</v>
       </c>
       <c r="M80" s="19">
@@ -12358,30 +12356,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -13564,22 +13562,22 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="31" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -14528,22 +14526,22 @@
       <c r="S43" s="4"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="32" t="s">
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -15366,22 +15364,22 @@
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="28" t="s">
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="30"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="30"/>
+      <c r="L67" s="30"/>
+      <c r="M67" s="31"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -16222,10 +16220,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706FE79C-A75D-4CCC-B6D5-819B78A840F5}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16233,23 +16231,20 @@
     <col min="1" max="1" width="28.140625" style="24" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="24"/>
     <col min="3" max="3" width="10.7109375" style="24" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="24"/>
-    <col min="6" max="6" width="16.85546875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="24" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="24"/>
+    <col min="4" max="4" width="16.85546875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -16258,32 +16253,24 @@
         <v>1</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>10</v>
       </c>
@@ -16294,19 +16281,13 @@
         <v>0.61</v>
       </c>
       <c r="D4" s="19">
-        <v>81002</v>
+        <v>1500000</v>
       </c>
       <c r="E4" s="19">
-        <v>166.63</v>
-      </c>
-      <c r="F4" s="19">
-        <v>1500000</v>
-      </c>
-      <c r="G4" s="19">
         <v>40.935000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>16</v>
       </c>
@@ -16317,19 +16298,13 @@
         <v>0.53</v>
       </c>
       <c r="D5" s="19">
-        <v>98582</v>
+        <v>2800</v>
       </c>
       <c r="E5" s="19">
-        <v>209.03</v>
-      </c>
-      <c r="F5" s="19">
-        <v>2800</v>
-      </c>
-      <c r="G5" s="19">
         <v>1341.6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>20</v>
       </c>
@@ -16340,19 +16315,13 @@
         <v>0.61</v>
       </c>
       <c r="D6" s="19">
-        <v>80752</v>
+        <v>97000</v>
       </c>
       <c r="E6" s="19">
-        <v>209.17</v>
-      </c>
-      <c r="F6" s="19">
-        <v>97000</v>
-      </c>
-      <c r="G6" s="19">
         <v>31.844999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>24</v>
       </c>
@@ -16363,32 +16332,24 @@
         <v>0.72</v>
       </c>
       <c r="D7" s="19">
-        <v>59386</v>
+        <v>700</v>
       </c>
       <c r="E7" s="19">
-        <v>159.51</v>
-      </c>
-      <c r="F7" s="19">
-        <v>700</v>
-      </c>
-      <c r="G7" s="19">
         <v>12094</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>11</v>
       </c>
@@ -16399,19 +16360,13 @@
         <v>0.87</v>
       </c>
       <c r="D9" s="19">
-        <v>6745.2</v>
+        <v>2000000</v>
       </c>
       <c r="E9" s="19">
-        <v>39.755000000000003</v>
-      </c>
-      <c r="F9" s="19">
-        <v>2000000</v>
-      </c>
-      <c r="G9" s="19">
         <v>28.872</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>16</v>
       </c>
@@ -16422,19 +16377,13 @@
         <v>0.84</v>
       </c>
       <c r="D10" s="19">
-        <v>8444.6</v>
+        <v>5900</v>
       </c>
       <c r="E10" s="19">
-        <v>47.363</v>
-      </c>
-      <c r="F10" s="19">
-        <v>5900</v>
-      </c>
-      <c r="G10" s="19">
         <v>1179.7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>20</v>
       </c>
@@ -16445,19 +16394,13 @@
         <v>0.87</v>
       </c>
       <c r="D11" s="19">
-        <v>6594.4</v>
+        <v>130000</v>
       </c>
       <c r="E11" s="19">
-        <v>43.311999999999998</v>
-      </c>
-      <c r="F11" s="19">
-        <v>130000</v>
-      </c>
-      <c r="G11" s="19">
         <v>34.655999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>23</v>
       </c>
@@ -16468,33 +16411,25 @@
         <v>0.88</v>
       </c>
       <c r="D12" s="19">
-        <v>6082.5</v>
+        <v>770</v>
       </c>
       <c r="E12" s="19">
-        <v>37.908000000000001</v>
-      </c>
-      <c r="F12" s="19">
-        <v>770</v>
-      </c>
-      <c r="G12" s="19">
         <v>10791</v>
       </c>
-      <c r="I12" s="41"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="27"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>11</v>
       </c>
@@ -16505,19 +16440,13 @@
         <v>0.87</v>
       </c>
       <c r="D14" s="19">
-        <v>67.085999999999999</v>
+        <v>2000000</v>
       </c>
       <c r="E14" s="19">
-        <v>5.9356</v>
-      </c>
-      <c r="F14" s="19">
-        <v>2000000</v>
-      </c>
-      <c r="G14" s="19">
         <v>7.7100999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>16</v>
       </c>
@@ -16528,19 +16457,13 @@
         <v>0.86</v>
       </c>
       <c r="D15" s="19">
-        <v>69.765000000000001</v>
+        <v>3400</v>
       </c>
       <c r="E15" s="19">
-        <v>5.9756</v>
-      </c>
-      <c r="F15" s="19">
-        <v>3400</v>
-      </c>
-      <c r="G15" s="19">
         <v>1207.0999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>20</v>
       </c>
@@ -16551,19 +16474,13 @@
         <v>0.88</v>
       </c>
       <c r="D16" s="19">
-        <v>62.377000000000002</v>
+        <v>140000</v>
       </c>
       <c r="E16" s="19">
-        <v>5.9661</v>
-      </c>
-      <c r="F16" s="19">
-        <v>140000</v>
-      </c>
-      <c r="G16" s="19">
         <v>22.919</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>23</v>
       </c>
@@ -16574,32 +16491,24 @@
         <v>0.88</v>
       </c>
       <c r="D17" s="19">
-        <v>61.453000000000003</v>
+        <v>1600</v>
       </c>
       <c r="E17" s="19">
-        <v>5.8826999999999998</v>
-      </c>
-      <c r="F17" s="19">
-        <v>1600</v>
-      </c>
-      <c r="G17" s="19">
         <v>3871.3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>12</v>
       </c>
@@ -16610,19 +16519,13 @@
         <v>0.87</v>
       </c>
       <c r="D19" s="19">
-        <v>5.6723999999999997</v>
+        <v>2100000</v>
       </c>
       <c r="E19" s="19">
-        <v>1.77</v>
-      </c>
-      <c r="F19" s="19">
-        <v>2100000</v>
-      </c>
-      <c r="G19" s="19">
         <v>1.8304</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>16</v>
       </c>
@@ -16633,19 +16536,13 @@
         <v>0.86</v>
       </c>
       <c r="D20" s="19">
-        <v>5.7961</v>
+        <v>2900</v>
       </c>
       <c r="E20" s="19">
-        <v>1.7283999999999999</v>
-      </c>
-      <c r="F20" s="19">
-        <v>2900</v>
-      </c>
-      <c r="G20" s="19">
         <v>1431.3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>20</v>
       </c>
@@ -16656,19 +16553,13 @@
         <v>0.87</v>
       </c>
       <c r="D21" s="19">
-        <v>5.2887000000000004</v>
+        <v>120000</v>
       </c>
       <c r="E21" s="19">
-        <v>1.7183999999999999</v>
-      </c>
-      <c r="F21" s="19">
-        <v>120000</v>
-      </c>
-      <c r="G21" s="19">
         <v>27.777999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>23</v>
       </c>
@@ -16679,29 +16570,21 @@
         <v>0.88</v>
       </c>
       <c r="D22" s="19">
-        <v>5.2008000000000001</v>
+        <v>1000</v>
       </c>
       <c r="E22" s="19">
-        <v>1.6979</v>
-      </c>
-      <c r="F22" s="19">
-        <v>1000</v>
-      </c>
-      <c r="G22" s="19">
         <v>5913.1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="40" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="26" t="s">
         <v>0</v>
@@ -16710,32 +16593,24 @@
         <v>1</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>10</v>
       </c>
@@ -16746,19 +16621,13 @@
         <v>0.63</v>
       </c>
       <c r="D27" s="19">
-        <v>73109</v>
+        <v>990000</v>
       </c>
       <c r="E27" s="19">
-        <v>160.55000000000001</v>
-      </c>
-      <c r="F27" s="19">
-        <v>990000</v>
-      </c>
-      <c r="G27" s="19">
         <v>4.6325000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>16</v>
       </c>
@@ -16769,19 +16638,13 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="D28" s="19">
-        <v>86585</v>
+        <v>8300</v>
       </c>
       <c r="E28" s="19">
-        <v>195.87</v>
-      </c>
-      <c r="F28" s="19">
-        <v>8300</v>
-      </c>
-      <c r="G28" s="19">
         <v>154.13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>20</v>
       </c>
@@ -16792,19 +16655,13 @@
         <v>0.6</v>
       </c>
       <c r="D29" s="19">
-        <v>80385</v>
+        <v>99000</v>
       </c>
       <c r="E29" s="19">
-        <v>215.78</v>
-      </c>
-      <c r="F29" s="19">
-        <v>99000</v>
-      </c>
-      <c r="G29" s="19">
         <v>8.4984999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>24</v>
       </c>
@@ -16815,32 +16672,24 @@
         <v>0.77</v>
       </c>
       <c r="D30" s="19">
-        <v>45018</v>
+        <v>2300</v>
       </c>
       <c r="E30" s="19">
-        <v>125.47</v>
-      </c>
-      <c r="F30" s="19">
-        <v>2300</v>
-      </c>
-      <c r="G30" s="19">
         <v>1729.1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>11</v>
       </c>
@@ -16851,19 +16700,13 @@
         <v>0.85</v>
       </c>
       <c r="D32" s="19">
-        <v>73.021000000000001</v>
+        <v>1700000</v>
       </c>
       <c r="E32" s="19">
-        <v>6.274</v>
-      </c>
-      <c r="F32" s="19">
-        <v>1700000</v>
-      </c>
-      <c r="G32" s="19">
         <v>0.84113000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>16</v>
       </c>
@@ -16874,19 +16717,13 @@
         <v>0.84</v>
       </c>
       <c r="D33" s="19">
-        <v>78.509</v>
+        <v>11000</v>
       </c>
       <c r="E33" s="19">
-        <v>6.3879999999999999</v>
-      </c>
-      <c r="F33" s="19">
-        <v>11000</v>
-      </c>
-      <c r="G33" s="19">
         <v>146.51</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>20</v>
       </c>
@@ -16897,19 +16734,13 @@
         <v>0.85</v>
       </c>
       <c r="D34" s="19">
-        <v>71.456999999999994</v>
+        <v>96000</v>
       </c>
       <c r="E34" s="19">
-        <v>6.6351000000000004</v>
-      </c>
-      <c r="F34" s="19">
-        <v>96000</v>
-      </c>
-      <c r="G34" s="19">
         <v>8.4078999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>23</v>
       </c>
@@ -16920,32 +16751,24 @@
         <v>0.86</v>
       </c>
       <c r="D35" s="19">
-        <v>67.468000000000004</v>
+        <v>2900</v>
       </c>
       <c r="E35" s="19">
-        <v>6.3014999999999999</v>
-      </c>
-      <c r="F35" s="19">
-        <v>2900</v>
-      </c>
-      <c r="G35" s="19">
         <v>695.62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>11</v>
       </c>
@@ -16956,19 +16779,13 @@
         <v>0.85</v>
       </c>
       <c r="D37" s="19">
-        <v>73.021000000000001</v>
+        <v>1700000</v>
       </c>
       <c r="E37" s="19">
-        <v>6.274</v>
-      </c>
-      <c r="F37" s="19">
-        <v>1700000</v>
-      </c>
-      <c r="G37" s="19">
         <v>0.84113000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>16</v>
       </c>
@@ -16979,19 +16796,13 @@
         <v>0.84</v>
       </c>
       <c r="D38" s="19">
-        <v>78.509</v>
+        <v>11000</v>
       </c>
       <c r="E38" s="19">
-        <v>6.3879999999999999</v>
-      </c>
-      <c r="F38" s="19">
-        <v>11000</v>
-      </c>
-      <c r="G38" s="19">
         <v>146.51</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>20</v>
       </c>
@@ -17002,19 +16813,13 @@
         <v>0.85</v>
       </c>
       <c r="D39" s="19">
-        <v>71.456999999999994</v>
+        <v>96000</v>
       </c>
       <c r="E39" s="19">
-        <v>6.6351000000000004</v>
-      </c>
-      <c r="F39" s="19">
-        <v>96000</v>
-      </c>
-      <c r="G39" s="19">
         <v>8.4078999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>23</v>
       </c>
@@ -17025,32 +16830,24 @@
         <v>0.86</v>
       </c>
       <c r="D40" s="19">
-        <v>67.468000000000004</v>
+        <v>2900</v>
       </c>
       <c r="E40" s="19">
-        <v>6.3014999999999999</v>
-      </c>
-      <c r="F40" s="19">
-        <v>2900</v>
-      </c>
-      <c r="G40" s="19">
         <v>695.62</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>11</v>
       </c>
@@ -17061,19 +16858,13 @@
         <v>0.86</v>
       </c>
       <c r="D42" s="19">
-        <v>5.8360000000000003</v>
+        <v>1600000</v>
       </c>
       <c r="E42" s="19">
-        <v>1.7770999999999999</v>
-      </c>
-      <c r="F42" s="19">
-        <v>1600000</v>
-      </c>
-      <c r="G42" s="19">
         <v>0.91227999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>16</v>
       </c>
@@ -17084,19 +16875,13 @@
         <v>0.85</v>
       </c>
       <c r="D43" s="19">
-        <v>6.0263</v>
+        <v>11000</v>
       </c>
       <c r="E43" s="19">
-        <v>1.7718</v>
-      </c>
-      <c r="F43" s="19">
-        <v>11000</v>
-      </c>
-      <c r="G43" s="19">
         <v>154.83000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>20</v>
       </c>
@@ -17107,19 +16892,13 @@
         <v>0.86</v>
       </c>
       <c r="D44" s="19">
-        <v>5.6726999999999999</v>
+        <v>88000</v>
       </c>
       <c r="E44" s="19">
-        <v>1.8119000000000001</v>
-      </c>
-      <c r="F44" s="19">
-        <v>88000</v>
-      </c>
-      <c r="G44" s="19">
         <v>7.5147000000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>23</v>
       </c>
@@ -17130,29 +16909,21 @@
         <v>0.87</v>
       </c>
       <c r="D45" s="19">
-        <v>5.3964999999999996</v>
+        <v>1600</v>
       </c>
       <c r="E45" s="19">
-        <v>1.7472000000000001</v>
-      </c>
-      <c r="F45" s="19">
-        <v>1600</v>
-      </c>
-      <c r="G45" s="19">
         <v>778.37</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="40" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="26" t="s">
         <v>0</v>
@@ -17161,32 +16932,24 @@
         <v>1</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="F48" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>10</v>
       </c>
@@ -17197,19 +16960,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="D50" s="19">
-        <v>86956</v>
+        <v>1000000</v>
       </c>
       <c r="E50" s="19">
-        <v>173.5</v>
-      </c>
-      <c r="F50" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="G50" s="19">
         <v>15.382</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>16</v>
       </c>
@@ -17219,20 +16976,14 @@
       <c r="C51" s="19">
         <v>0.51</v>
       </c>
-      <c r="D51" s="27">
-        <v>100820</v>
+      <c r="D51" s="19">
+        <v>5000</v>
       </c>
       <c r="E51" s="19">
-        <v>211.94</v>
-      </c>
-      <c r="F51" s="19">
-        <v>5000</v>
-      </c>
-      <c r="G51" s="19">
         <v>401.97</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>20</v>
       </c>
@@ -17243,19 +16994,13 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="D52" s="19">
-        <v>89618</v>
+        <v>100000</v>
       </c>
       <c r="E52" s="19">
-        <v>224.81</v>
-      </c>
-      <c r="F52" s="19">
-        <v>100000</v>
-      </c>
-      <c r="G52" s="19">
         <v>13.547000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>24</v>
       </c>
@@ -17266,32 +17011,24 @@
         <v>0.72</v>
       </c>
       <c r="D53" s="19">
-        <v>57644</v>
+        <v>1200</v>
       </c>
       <c r="E53" s="19">
-        <v>147.31</v>
-      </c>
-      <c r="F53" s="19">
-        <v>1200</v>
-      </c>
-      <c r="G53" s="19">
         <v>3970.6</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>10</v>
       </c>
@@ -17302,19 +17039,13 @@
         <v>0.87</v>
       </c>
       <c r="D55" s="19">
-        <v>66.091999999999999</v>
+        <v>2000000</v>
       </c>
       <c r="E55" s="19">
-        <v>5.8639000000000001</v>
-      </c>
-      <c r="F55" s="19">
-        <v>2000000</v>
-      </c>
-      <c r="G55" s="19">
         <v>1.8412999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>16</v>
       </c>
@@ -17325,19 +17056,13 @@
         <v>0.87</v>
       </c>
       <c r="D56" s="19">
-        <v>68.057000000000002</v>
+        <v>7100</v>
       </c>
       <c r="E56" s="19">
-        <v>5.867</v>
-      </c>
-      <c r="F56" s="19">
-        <v>7100</v>
-      </c>
-      <c r="G56" s="19">
         <v>301.2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>20</v>
       </c>
@@ -17348,19 +17073,13 @@
         <v>0.88</v>
       </c>
       <c r="D57" s="19">
-        <v>63.003</v>
+        <v>150000</v>
       </c>
       <c r="E57" s="19">
-        <v>6.0275999999999996</v>
-      </c>
-      <c r="F57" s="19">
-        <v>150000</v>
-      </c>
-      <c r="G57" s="19">
         <v>8.7688000000000006</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>23</v>
       </c>
@@ -17371,32 +17090,24 @@
         <v>0.88</v>
       </c>
       <c r="D58" s="19">
-        <v>60.606000000000002</v>
+        <v>2200</v>
       </c>
       <c r="E58" s="19">
-        <v>5.82</v>
-      </c>
-      <c r="F58" s="19">
-        <v>2200</v>
-      </c>
-      <c r="G58" s="19">
         <v>1505</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B59" s="39" t="s">
+      <c r="B59" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>11</v>
       </c>
@@ -17407,19 +17118,13 @@
         <v>0.87</v>
       </c>
       <c r="D60" s="19">
-        <v>66.091999999999999</v>
+        <v>2000000</v>
       </c>
       <c r="E60" s="19">
-        <v>5.8639000000000001</v>
-      </c>
-      <c r="F60" s="19">
-        <v>2000000</v>
-      </c>
-      <c r="G60" s="19">
         <v>1.8412999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>16</v>
       </c>
@@ -17430,19 +17135,13 @@
         <v>0.87</v>
       </c>
       <c r="D61" s="19">
-        <v>68.057000000000002</v>
+        <v>7100</v>
       </c>
       <c r="E61" s="19">
-        <v>5.867</v>
-      </c>
-      <c r="F61" s="19">
-        <v>7100</v>
-      </c>
-      <c r="G61" s="19">
         <v>301.2</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>20</v>
       </c>
@@ -17453,19 +17152,13 @@
         <v>0.88</v>
       </c>
       <c r="D62" s="19">
-        <v>63.003</v>
+        <v>150000</v>
       </c>
       <c r="E62" s="19">
-        <v>6.0275999999999996</v>
-      </c>
-      <c r="F62" s="19">
-        <v>150000</v>
-      </c>
-      <c r="G62" s="19">
         <v>8.7688000000000006</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>23</v>
       </c>
@@ -17476,32 +17169,24 @@
         <v>0.88</v>
       </c>
       <c r="D63" s="19">
-        <v>60.606000000000002</v>
+        <v>2200</v>
       </c>
       <c r="E63" s="19">
-        <v>5.82</v>
-      </c>
-      <c r="F63" s="19">
-        <v>2200</v>
-      </c>
-      <c r="G63" s="19">
         <v>1505</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B64" s="39" t="s">
+      <c r="B64" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>39</v>
       </c>
@@ -17512,19 +17197,13 @@
         <v>0.87</v>
       </c>
       <c r="D65" s="19">
-        <v>5.5647000000000002</v>
+        <v>1600000</v>
       </c>
       <c r="E65" s="19">
-        <v>1.7563</v>
-      </c>
-      <c r="F65" s="19">
-        <v>1600000</v>
-      </c>
-      <c r="G65" s="19">
         <v>0.81047999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>16</v>
       </c>
@@ -17535,19 +17214,13 @@
         <v>0.86</v>
       </c>
       <c r="D66" s="19">
-        <v>5.7131999999999996</v>
+        <v>3600</v>
       </c>
       <c r="E66" s="19">
-        <v>1.72</v>
-      </c>
-      <c r="F66" s="19">
-        <v>3600</v>
-      </c>
-      <c r="G66" s="19">
         <v>521.98</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
         <v>20</v>
       </c>
@@ -17558,19 +17231,13 @@
         <v>0.87</v>
       </c>
       <c r="D67" s="19">
-        <v>5.3757999999999999</v>
+        <v>99000</v>
       </c>
       <c r="E67" s="19">
-        <v>1.7385999999999999</v>
-      </c>
-      <c r="F67" s="19">
-        <v>99000</v>
-      </c>
-      <c r="G67" s="19">
         <v>14.904</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
         <v>23</v>
       </c>
@@ -17581,29 +17248,21 @@
         <v>0.88</v>
       </c>
       <c r="D68" s="19">
-        <v>5.1988000000000003</v>
+        <v>1600</v>
       </c>
       <c r="E68" s="19">
-        <v>1.6978</v>
-      </c>
-      <c r="F68" s="19">
-        <v>1600</v>
-      </c>
-      <c r="G68" s="19">
         <v>1878</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="40" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="40"/>
-      <c r="G70" s="40"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C70" s="41"/>
+      <c r="D70" s="41"/>
+      <c r="E70" s="41"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
       <c r="B71" s="26" t="s">
         <v>0</v>
@@ -17612,32 +17271,24 @@
         <v>1</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E71" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="F71" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G71" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B72" s="39" t="s">
+      <c r="B72" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
-      <c r="G72" s="39"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
         <v>10</v>
       </c>
@@ -17647,20 +17298,14 @@
       <c r="C73" s="19">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D73" s="27">
-        <v>115180</v>
+      <c r="D73" s="19">
+        <v>520000</v>
       </c>
       <c r="E73" s="19">
-        <v>203.26</v>
-      </c>
-      <c r="F73" s="19">
-        <v>520000</v>
-      </c>
-      <c r="G73" s="19">
         <v>0.57515000000000005</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
         <v>16</v>
       </c>
@@ -17670,20 +17315,14 @@
       <c r="C74" s="19">
         <v>0.5</v>
       </c>
-      <c r="D74" s="27">
-        <v>125630</v>
+      <c r="D74" s="19">
+        <v>29000</v>
       </c>
       <c r="E74" s="19">
-        <v>231.99</v>
-      </c>
-      <c r="F74" s="19">
-        <v>29000</v>
-      </c>
-      <c r="G74" s="19">
         <v>13.69</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
         <v>20</v>
       </c>
@@ -17693,20 +17332,14 @@
       <c r="C75" s="19">
         <v>0.41</v>
       </c>
-      <c r="D75" s="27">
-        <v>150730</v>
+      <c r="D75" s="19">
+        <v>47000</v>
       </c>
       <c r="E75" s="19">
-        <v>302.11</v>
-      </c>
-      <c r="F75" s="19">
-        <v>47000</v>
-      </c>
-      <c r="G75" s="19">
         <v>3.1452</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>23</v>
       </c>
@@ -17717,32 +17350,24 @@
         <v>0.79</v>
       </c>
       <c r="D76" s="19">
-        <v>54387</v>
+        <v>7900</v>
       </c>
       <c r="E76" s="19">
-        <v>141.18</v>
-      </c>
-      <c r="F76" s="19">
-        <v>7900</v>
-      </c>
-      <c r="G76" s="19">
         <v>143.07</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B77" s="39" t="s">
+      <c r="B77" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="39"/>
-      <c r="G77" s="39"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C77" s="40"/>
+      <c r="D77" s="40"/>
+      <c r="E77" s="40"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>11</v>
       </c>
@@ -17753,19 +17378,13 @@
         <v>0.86</v>
       </c>
       <c r="D78" s="19">
-        <v>68.341999999999999</v>
+        <v>700000</v>
       </c>
       <c r="E78" s="19">
-        <v>5.9093</v>
-      </c>
-      <c r="F78" s="19">
-        <v>700000</v>
-      </c>
-      <c r="G78" s="19">
         <v>0.19005</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>16</v>
       </c>
@@ -17776,19 +17395,13 @@
         <v>0.86</v>
       </c>
       <c r="D79" s="19">
-        <v>68.245999999999995</v>
+        <v>43000</v>
       </c>
       <c r="E79" s="19">
-        <v>5.7678000000000003</v>
-      </c>
-      <c r="F79" s="19">
-        <v>43000</v>
-      </c>
-      <c r="G79" s="19">
         <v>9.0985999999999994</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>19</v>
       </c>
@@ -17799,19 +17412,13 @@
         <v>0.82</v>
       </c>
       <c r="D80" s="19">
-        <v>89.632000000000005</v>
+        <v>110000</v>
       </c>
       <c r="E80" s="19">
-        <v>7.7064000000000004</v>
-      </c>
-      <c r="F80" s="19">
-        <v>110000</v>
-      </c>
-      <c r="G80" s="19">
         <v>1.4948999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
         <v>23</v>
       </c>
@@ -17822,32 +17429,24 @@
         <v>0.88</v>
       </c>
       <c r="D81" s="19">
-        <v>61.058</v>
+        <v>11000</v>
       </c>
       <c r="E81" s="19">
-        <v>5.6593999999999998</v>
-      </c>
-      <c r="F81" s="19">
-        <v>11000</v>
-      </c>
-      <c r="G81" s="19">
         <v>82.043999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B82" s="39" t="s">
+      <c r="B82" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
-      <c r="F82" s="39"/>
-      <c r="G82" s="39"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C82" s="40"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="40"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
         <v>11</v>
       </c>
@@ -17858,19 +17457,13 @@
         <v>0.86</v>
       </c>
       <c r="D83" s="19">
-        <v>68.341999999999999</v>
+        <v>700000</v>
       </c>
       <c r="E83" s="19">
-        <v>5.9093</v>
-      </c>
-      <c r="F83" s="19">
-        <v>700000</v>
-      </c>
-      <c r="G83" s="19">
         <v>0.19005</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>16</v>
       </c>
@@ -17881,19 +17474,13 @@
         <v>0.86</v>
       </c>
       <c r="D84" s="19">
-        <v>68.245999999999995</v>
+        <v>43000</v>
       </c>
       <c r="E84" s="19">
-        <v>5.7678000000000003</v>
-      </c>
-      <c r="F84" s="19">
-        <v>43000</v>
-      </c>
-      <c r="G84" s="19">
         <v>9.0985999999999994</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>19</v>
       </c>
@@ -17904,19 +17491,13 @@
         <v>0.82</v>
       </c>
       <c r="D85" s="19">
-        <v>89.632000000000005</v>
+        <v>110000</v>
       </c>
       <c r="E85" s="19">
-        <v>7.7064000000000004</v>
-      </c>
-      <c r="F85" s="19">
-        <v>110000</v>
-      </c>
-      <c r="G85" s="19">
         <v>1.4948999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
         <v>23</v>
       </c>
@@ -17927,32 +17508,24 @@
         <v>0.88</v>
       </c>
       <c r="D86" s="19">
-        <v>61.058</v>
+        <v>11000</v>
       </c>
       <c r="E86" s="19">
-        <v>5.6593999999999998</v>
-      </c>
-      <c r="F86" s="19">
-        <v>11000</v>
-      </c>
-      <c r="G86" s="19">
         <v>82.043999999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B87" s="39" t="s">
+      <c r="B87" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C87" s="39"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="39"/>
-      <c r="F87" s="39"/>
-      <c r="G87" s="39"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="40"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
         <v>11</v>
       </c>
@@ -17963,19 +17536,13 @@
         <v>0.83</v>
       </c>
       <c r="D88" s="19">
-        <v>8.0870999999999995</v>
+        <v>660000</v>
       </c>
       <c r="E88" s="19">
-        <v>2.1181000000000001</v>
-      </c>
-      <c r="F88" s="19">
-        <v>660000</v>
-      </c>
-      <c r="G88" s="19">
         <v>0.21106</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
         <v>16</v>
       </c>
@@ -17986,19 +17553,13 @@
         <v>0.83</v>
       </c>
       <c r="D89" s="19">
-        <v>8.1913</v>
+        <v>31000</v>
       </c>
       <c r="E89" s="19">
-        <v>2.0590000000000002</v>
-      </c>
-      <c r="F89" s="19">
-        <v>31000</v>
-      </c>
-      <c r="G89" s="19">
         <v>10.798</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>19</v>
       </c>
@@ -18009,19 +17570,13 @@
         <v>0.8</v>
       </c>
       <c r="D90" s="19">
-        <v>9.2324999999999999</v>
+        <v>110000</v>
       </c>
       <c r="E90" s="19">
-        <v>2.4870000000000001</v>
-      </c>
-      <c r="F90" s="19">
-        <v>110000</v>
-      </c>
-      <c r="G90" s="19">
         <v>1.4992000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
         <v>23</v>
       </c>
@@ -18032,40 +17587,34 @@
         <v>0.84</v>
       </c>
       <c r="D91" s="19">
-        <v>7.2984999999999998</v>
+        <v>6500</v>
       </c>
       <c r="E91" s="19">
-        <v>2.0457999999999998</v>
-      </c>
-      <c r="F91" s="19">
-        <v>6500</v>
-      </c>
-      <c r="G91" s="19">
         <v>122.94</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B82:G82"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B77:E77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>